<commit_message>
Refactor code, create uml, finish documentation
</commit_message>
<xml_diff>
--- a/results/everything.xlsx
+++ b/results/everything.xlsx
@@ -527,31 +527,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -581,6 +560,45 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -605,24 +623,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -657,8 +657,9 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -675,17 +676,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -719,7 +718,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -736,17 +734,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -780,7 +776,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -797,17 +792,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -841,7 +834,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -858,17 +850,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -902,7 +892,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -912,17 +901,78 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="-148867488"/>
-        <c:axId val="-148858240"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1969833984"/>
+        <c:axId val="-1969824736"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="-148867488"/>
+        <c:axId val="-1969833984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>Tanítóhalmaz mérete</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="hu-HU" baseline="0"/>
+                  <a:t> (cikk/író)</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -960,7 +1010,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-148858240"/>
+        <c:crossAx val="-1969824736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -968,7 +1018,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-148858240"/>
+        <c:axId val="-1969824736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -988,6 +1038,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>F-mérték</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1019,7 +1125,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-148867488"/>
+        <c:crossAx val="-1969833984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1117,8 +1223,9 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1135,17 +1242,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -1179,7 +1284,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1196,17 +1300,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -1240,7 +1342,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1257,17 +1358,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -1301,7 +1400,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1318,17 +1416,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
@@ -1362,7 +1458,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1372,17 +1467,73 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="-1585062928"/>
-        <c:axId val="-1585078160"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1969828000"/>
+        <c:axId val="-1969829632"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="-1585062928"/>
+        <c:axId val="-1969828000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>Tanítóhalmaz mérete (cikk/író)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1420,7 +1571,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1585078160"/>
+        <c:crossAx val="-1969829632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1428,7 +1579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1585078160"/>
+        <c:axId val="-1969829632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,6 +1599,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>F-mérték</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1479,7 +1686,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1585062928"/>
+        <c:crossAx val="-1969828000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1577,8 +1784,9 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1595,17 +1803,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Munka1!$C$32:$E$32</c:f>
@@ -1642,7 +1848,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1659,17 +1864,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Munka1!$C$32:$E$32</c:f>
@@ -1706,7 +1909,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1723,17 +1925,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Munka1!$C$32:$E$32</c:f>
@@ -1770,7 +1970,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1787,17 +1986,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Munka1!$C$32:$E$32</c:f>
@@ -1834,7 +2031,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1844,17 +2040,78 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="-1676629504"/>
-        <c:axId val="-1676630592"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1969823648"/>
+        <c:axId val="-1969835616"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="-1676629504"/>
+        <c:axId val="-1969823648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>Frekvencia</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="hu-HU" baseline="0"/>
+                  <a:t> alapú vágási határ(%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1892,7 +2149,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676630592"/>
+        <c:crossAx val="-1969835616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1900,7 +2157,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676630592"/>
+        <c:axId val="-1969835616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1922,6 +2179,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>F-mérték</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1953,7 +2266,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676629504"/>
+        <c:crossAx val="-1969823648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2051,8 +2364,9 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2069,17 +2383,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Munka1!$C$48:$E$48</c:f>
@@ -2116,7 +2428,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2133,17 +2444,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Munka1!$C$48:$E$48</c:f>
@@ -2180,7 +2489,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2197,17 +2505,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Munka1!$C$48:$E$48</c:f>
@@ -2244,7 +2550,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2261,17 +2566,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Munka1!$C$48:$E$48</c:f>
@@ -2308,7 +2611,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2318,17 +2620,78 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="-1676616992"/>
-        <c:axId val="-1676624064"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1969823104"/>
+        <c:axId val="-1969822560"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="-1676616992"/>
+        <c:axId val="-1969823104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>Frekvencia</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="hu-HU" baseline="0"/>
+                  <a:t> alapú vágási határ(%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2366,7 +2729,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676624064"/>
+        <c:crossAx val="-1969822560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2374,7 +2737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1676624064"/>
+        <c:axId val="-1969822560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2396,6 +2759,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>F-mérték</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2427,7 +2846,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1676616992"/>
+        <c:crossAx val="-1969823104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2656,11 +3075,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-148857696"/>
-        <c:axId val="-148856064"/>
+        <c:axId val="-1969822016"/>
+        <c:axId val="-1969837248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-148857696"/>
+        <c:axId val="-1969822016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2703,7 +3122,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-148856064"/>
+        <c:crossAx val="-1969837248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2711,7 +3130,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-148856064"/>
+        <c:axId val="-1969837248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2762,7 +3181,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-148857696"/>
+        <c:crossAx val="-1969822016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2972,11 +3391,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-148859872"/>
-        <c:axId val="-148862048"/>
+        <c:axId val="-1928900128"/>
+        <c:axId val="-1928893600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-148859872"/>
+        <c:axId val="-1928900128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3019,7 +3438,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-148862048"/>
+        <c:crossAx val="-1928893600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3027,7 +3446,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-148862048"/>
+        <c:axId val="-1928893600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3078,7 +3497,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-148859872"/>
+        <c:crossAx val="-1928900128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6924,8 +7343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79:C84"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6941,13 +7360,13 @@
       <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="44">
+      <c r="C1" s="13">
         <v>0.70531128921419961</v>
       </c>
-      <c r="D1" s="44">
+      <c r="D1" s="13">
         <v>0.77232327581496751</v>
       </c>
-      <c r="E1" s="44">
+      <c r="E1" s="13">
         <v>0.84150692258711479</v>
       </c>
     </row>
@@ -6955,13 +7374,13 @@
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="14">
         <v>0.34723914582740822</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="14">
         <v>0.59262628524366501</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="14">
         <v>0.73687540183684608</v>
       </c>
     </row>
@@ -6969,13 +7388,13 @@
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="14">
         <v>0.52256499763653175</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="14">
         <v>0.6293639171898906</v>
       </c>
-      <c r="E3" s="45">
+      <c r="E3" s="14">
         <v>0.7382253321911757</v>
       </c>
     </row>
@@ -6983,13 +7402,13 @@
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="14">
         <v>0.20890457133112708</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="14">
         <v>0.44473654217603925</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="14">
         <v>0.60480575478760534</v>
       </c>
     </row>
@@ -7000,13 +7419,13 @@
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="14">
         <v>0.89368269218764251</v>
       </c>
-      <c r="D18" s="45">
+      <c r="D18" s="14">
         <v>0.91764424998963601</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="14">
         <v>0.94792326860334952</v>
       </c>
     </row>
@@ -7014,13 +7433,13 @@
       <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="14">
         <v>0.35676264442579114</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D19" s="14">
         <v>0.6479003957099787</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="14">
         <v>0.78369969934774653</v>
       </c>
     </row>
@@ -7028,13 +7447,13 @@
       <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="14">
         <v>0.52305380128122891</v>
       </c>
-      <c r="D20" s="45">
+      <c r="D20" s="14">
         <v>0.62714215408485618</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="14">
         <v>0.74092451402219806</v>
       </c>
     </row>
@@ -7042,13 +7461,13 @@
       <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="14">
         <v>0.20075543213517502</v>
       </c>
-      <c r="D21" s="45">
+      <c r="D21" s="14">
         <v>0.43990095455860467</v>
       </c>
-      <c r="E21" s="45">
+      <c r="E21" s="14">
         <v>0.60508770917246524</v>
       </c>
     </row>
@@ -7070,13 +7489,13 @@
       <c r="B33" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="45">
+      <c r="C33" s="14">
         <v>0.70531128921419961</v>
       </c>
-      <c r="D33" s="45">
+      <c r="D33" s="14">
         <v>0.89368269218764251</v>
       </c>
-      <c r="E33" s="45">
+      <c r="E33" s="14">
         <v>0.97620094212580943</v>
       </c>
     </row>
@@ -7084,13 +7503,13 @@
       <c r="B34" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="45">
+      <c r="C34" s="14">
         <v>0.34723914582740822</v>
       </c>
-      <c r="D34" s="45">
+      <c r="D34" s="14">
         <v>0.35676264442579114</v>
       </c>
-      <c r="E34" s="45">
+      <c r="E34" s="14">
         <v>0.25589509485597628</v>
       </c>
     </row>
@@ -7098,13 +7517,13 @@
       <c r="B35" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="45">
+      <c r="C35" s="14">
         <v>0.52256499763653175</v>
       </c>
-      <c r="D35" s="45">
+      <c r="D35" s="14">
         <v>0.52305380128122891</v>
       </c>
-      <c r="E35" s="45">
+      <c r="E35" s="14">
         <v>0.56889394000119409</v>
       </c>
     </row>
@@ -7112,13 +7531,13 @@
       <c r="B36" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="45">
+      <c r="C36" s="14">
         <v>0.20890457133112708</v>
       </c>
-      <c r="D36" s="45">
+      <c r="D36" s="14">
         <v>0.20075543213517502</v>
       </c>
-      <c r="E36" s="45">
+      <c r="E36" s="14">
         <v>0.20875431764346375</v>
       </c>
     </row>
@@ -7140,13 +7559,13 @@
       <c r="B49" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="45">
+      <c r="C49" s="14">
         <v>0.84150692258711479</v>
       </c>
-      <c r="D49" s="45">
+      <c r="D49" s="14">
         <v>0.94792326860334952</v>
       </c>
-      <c r="E49" s="45">
+      <c r="E49" s="14">
         <v>0.98935458965722822</v>
       </c>
     </row>
@@ -7154,13 +7573,13 @@
       <c r="B50" t="s">
         <v>16</v>
       </c>
-      <c r="C50" s="45">
+      <c r="C50" s="14">
         <v>0.73687540183684608</v>
       </c>
-      <c r="D50" s="45">
+      <c r="D50" s="14">
         <v>0.78369969934774653</v>
       </c>
-      <c r="E50" s="45">
+      <c r="E50" s="14">
         <v>0.63761107467158884</v>
       </c>
     </row>
@@ -7168,13 +7587,13 @@
       <c r="B51" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="45">
+      <c r="C51" s="14">
         <v>0.7382253321911757</v>
       </c>
-      <c r="D51" s="45">
+      <c r="D51" s="14">
         <v>0.74092451402219806</v>
       </c>
-      <c r="E51" s="45">
+      <c r="E51" s="14">
         <v>0.76496873172409885</v>
       </c>
     </row>
@@ -7182,13 +7601,13 @@
       <c r="B52" t="s">
         <v>21</v>
       </c>
-      <c r="C52" s="45">
+      <c r="C52" s="14">
         <v>0.60480575478760534</v>
       </c>
-      <c r="D52" s="45">
+      <c r="D52" s="14">
         <v>0.60508770917246524</v>
       </c>
-      <c r="E52" s="45">
+      <c r="E52" s="14">
         <v>0.61823673970632609</v>
       </c>
     </row>
@@ -7207,10 +7626,10 @@
       <c r="B65" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="45">
+      <c r="C65" s="14">
         <v>0.91764424998963601</v>
       </c>
-      <c r="D65" s="45">
+      <c r="D65" s="14">
         <v>0.84918584030581756</v>
       </c>
     </row>
@@ -7218,20 +7637,20 @@
       <c r="B66" t="s">
         <v>16</v>
       </c>
-      <c r="C66" s="45">
+      <c r="C66" s="14">
         <v>0.6479003957099787</v>
       </c>
-      <c r="D66" s="45">
+      <c r="D66" s="14">
         <v>0.65016623192766754</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C67" s="45"/>
-      <c r="D67" s="45"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C68" s="45"/>
-      <c r="D68" s="45"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -7240,37 +7659,37 @@
       <c r="B79" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="46">
+      <c r="C79" s="15">
         <v>0.94792326860334952</v>
       </c>
-      <c r="D79" s="45"/>
-      <c r="E79" s="45"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>16</v>
       </c>
-      <c r="C80" s="46">
+      <c r="C80" s="15">
         <v>0.74092451402219806</v>
       </c>
-      <c r="D80" s="45"/>
-      <c r="E80" s="45"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>23</v>
       </c>
-      <c r="C81" s="46">
+      <c r="C81" s="15">
         <v>0.13772090188909203</v>
       </c>
-      <c r="D81" s="45"/>
-      <c r="E81" s="45"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="46">
+      <c r="C82" s="15">
         <v>0.76496873172409885</v>
       </c>
     </row>
@@ -7278,7 +7697,7 @@
       <c r="B83" t="s">
         <v>21</v>
       </c>
-      <c r="C83" s="46">
+      <c r="C83" s="15">
         <v>0.60508770917246524</v>
       </c>
     </row>
@@ -7286,7 +7705,7 @@
       <c r="B84" t="s">
         <v>24</v>
       </c>
-      <c r="C84" s="46">
+      <c r="C84" s="15">
         <v>0.1386584165377584</v>
       </c>
     </row>
@@ -7307,96 +7726,96 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="14" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="16"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="28"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="17" t="s">
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="19"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="31"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="20" t="s">
+      <c r="R2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="21"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="33"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="25"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="20"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="24"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="19"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-      <c r="S3" s="22" t="s">
+      <c r="S3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="25"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="20"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -7667,68 +8086,68 @@
       <c r="V8" s="7"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="26" t="s">
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="28"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="23"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="29" t="s">
+      <c r="R9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="30"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="25"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="25"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="24"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="19"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="22" t="s">
+      <c r="S10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="25"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="20"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -7999,68 +8418,68 @@
       <c r="V15" s="7"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="8"/>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="26" t="s">
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="28"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="23"/>
       <c r="Q16" s="8"/>
-      <c r="R16" s="29" t="s">
+      <c r="R16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="30"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="22"/>
+      <c r="V16" s="25"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="25"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="20"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="22" t="s">
+      <c r="M17" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="24"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="19"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="22" t="s">
+      <c r="S17" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
-      <c r="V17" s="25"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="20"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -8307,34 +8726,34 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="G23" s="13" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="G23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13" t="s">
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="R23" s="13" t="s">
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="R23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -8610,20 +9029,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="L23:P23"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="S10:V10"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="L16:P16"/>
-    <mergeCell ref="R16:V16"/>
     <mergeCell ref="R23:V23"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="L1:V1"/>
@@ -8640,6 +9045,20 @@
     <mergeCell ref="L9:P9"/>
     <mergeCell ref="R9:V9"/>
     <mergeCell ref="S17:V17"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="S10:V10"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="L16:P16"/>
+    <mergeCell ref="R16:V16"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="L23:P23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8662,96 +9081,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="34" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="41"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38" t="s">
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="36" t="s">
+      <c r="R2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="37"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="45"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="40"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-      <c r="S3" s="39" t="s">
+      <c r="S3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="40"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="35"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -9022,68 +9441,68 @@
       <c r="V8" s="7"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="28" t="s">
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="42" t="s">
+      <c r="R9" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="S9" s="42"/>
-      <c r="T9" s="42"/>
-      <c r="U9" s="42"/>
-      <c r="V9" s="43"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="38"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="40"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="35"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="39" t="s">
+      <c r="S10" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="T10" s="39"/>
-      <c r="U10" s="39"/>
-      <c r="V10" s="40"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34"/>
+      <c r="V10" s="35"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -9354,68 +9773,68 @@
       <c r="V15" s="7"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="8"/>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="41" t="s">
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
       <c r="Q16" s="8"/>
-      <c r="R16" s="42" t="s">
+      <c r="R16" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
-      <c r="U16" s="42"/>
-      <c r="V16" s="43"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="38"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="35"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="39" t="s">
+      <c r="M17" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
-      <c r="S17" s="39" t="s">
+      <c r="S17" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="T17" s="39"/>
-      <c r="U17" s="39"/>
-      <c r="V17" s="40"/>
+      <c r="T17" s="34"/>
+      <c r="U17" s="34"/>
+      <c r="V17" s="35"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -9662,34 +10081,34 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="G23" s="13" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="G23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13" t="s">
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="R23" s="13" t="s">
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="R23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -9971,6 +10390,28 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="L1:V1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="S3:V3"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="R9:V9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="S10:V10"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="L16:P16"/>
+    <mergeCell ref="R16:V16"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="G23:K23"/>
     <mergeCell ref="L23:P23"/>
@@ -9979,28 +10420,6 @@
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="M17:P17"/>
     <mergeCell ref="S17:V17"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="S10:V10"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="L16:P16"/>
-    <mergeCell ref="R16:V16"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="R9:V9"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="L1:V1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="R2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10021,96 +10440,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="34" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="41"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="38" t="s">
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="36" t="s">
+      <c r="R2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="37"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="45"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="40"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
-      <c r="S3" s="39" t="s">
+      <c r="S3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="40"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="35"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>

</xml_diff>